<commit_message>
added support for saving the `xlr_n_percent` to excel. At this point it is the most simple design, we convert it to a character and save it.
</commit_message>
<xml_diff>
--- a/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
+++ b/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">test_r_numeric</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">test_r_complex</t>
   </si>
   <si>
+    <t xml:space="preserve">test_xlr_n_percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
@@ -53,7 +56,103 @@
     <t xml:space="preserve">1+1i</t>
   </si>
   <si>
+    <t xml:space="preserve">1 (3%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (12%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (16%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (19%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 (22%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 (25%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 (28%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 (31%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 (34%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 (38%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 (41%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (44%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 (47%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (50%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 (53%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (56%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 (59%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (62%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 (66%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 (69%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 (72%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 (75%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 (78%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 (81%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (84%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 (88%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 (91%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 (94%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (97%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 (100%)</t>
   </si>
 </sst>
 </file>
@@ -103,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -127,6 +226,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -453,6 +555,9 @@
       <c r="J2" t="s">
         <v>9</v>
       </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -474,16 +579,19 @@
         <v>2.62</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="8" t="n">
         <v>16.46</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +614,19 @@
         <v>2.875</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +649,19 @@
         <v>2.32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>18.61</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -570,16 +684,19 @@
         <v>3.215</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="8" t="n">
         <v>19.44</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -602,16 +719,19 @@
         <v>3.44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -634,16 +754,19 @@
         <v>3.46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="8" t="n">
         <v>20.22</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -666,16 +789,19 @@
         <v>3.57</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" s="8" t="n">
         <v>15.84</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -698,16 +824,19 @@
         <v>3.19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H10" s="8" t="n">
         <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -730,16 +859,19 @@
         <v>3.15</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="8" t="n">
         <v>22.9</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -762,16 +894,19 @@
         <v>3.44</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="8" t="n">
         <v>18.3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -794,16 +929,19 @@
         <v>3.44</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -826,16 +964,19 @@
         <v>4.07</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H14" s="8" t="n">
         <v>17.4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15">
@@ -858,16 +999,19 @@
         <v>3.73</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15" s="8" t="n">
         <v>17.6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -890,16 +1034,19 @@
         <v>3.78</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16" s="8" t="n">
         <v>18</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17">
@@ -922,16 +1069,19 @@
         <v>5.25</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="8" t="n">
         <v>17.98</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -954,16 +1104,19 @@
         <v>5.424</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18" s="8" t="n">
         <v>17.82</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19">
@@ -986,16 +1139,19 @@
         <v>5.345</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="8" t="n">
         <v>17.42</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20">
@@ -1018,16 +1174,19 @@
         <v>2.2</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="8" t="n">
         <v>19.47</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21">
@@ -1050,16 +1209,19 @@
         <v>1.615</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21" s="8" t="n">
         <v>18.52</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22">
@@ -1082,16 +1244,19 @@
         <v>1.835</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H22" s="8" t="n">
         <v>19.9</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23">
@@ -1114,16 +1279,19 @@
         <v>2.465</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H23" s="8" t="n">
         <v>20.01</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24">
@@ -1146,16 +1314,19 @@
         <v>3.52</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24" s="8" t="n">
         <v>16.87</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25">
@@ -1178,16 +1349,19 @@
         <v>3.435</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25" s="8" t="n">
         <v>17.3</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26">
@@ -1210,16 +1384,19 @@
         <v>3.84</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H26" s="8" t="n">
         <v>15.41</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27">
@@ -1242,16 +1419,19 @@
         <v>3.845</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H27" s="8" t="n">
         <v>17.05</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28">
@@ -1274,16 +1454,19 @@
         <v>1.935</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H28" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29">
@@ -1306,16 +1489,19 @@
         <v>2.14</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29" s="8" t="n">
         <v>16.7</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30">
@@ -1338,16 +1524,19 @@
         <v>1.513</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30" s="8" t="n">
         <v>16.9</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31">
@@ -1370,16 +1559,19 @@
         <v>3.17</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H31" s="8" t="n">
         <v>14.5</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32">
@@ -1402,16 +1594,19 @@
         <v>2.77</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H32" s="8" t="n">
         <v>15.5</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33">
@@ -1434,16 +1629,19 @@
         <v>3.57</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H33" s="8" t="n">
         <v>14.6</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34">
@@ -1466,16 +1664,19 @@
         <v>2.78</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H34" s="8" t="n">
         <v>18.6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35">
@@ -1489,6 +1690,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
+      <c r="K35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added column widths to xlr_format
</commit_message>
<xml_diff>
--- a/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
+++ b/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">test_r_numeric</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">test_r_complex</t>
   </si>
   <si>
-    <t xml:space="preserve">test_xlr_n_percent</t>
-  </si>
-  <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
@@ -56,103 +53,7 @@
     <t xml:space="preserve">1+1i</t>
   </si>
   <si>
-    <t xml:space="preserve">1 (3%)</t>
-  </si>
-  <si>
     <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 (6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 (9%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 (12%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 (16%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 (19%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7 (22%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 (25%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (28%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 (31%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 (34%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 (38%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (41%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 (44%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 (47%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (50%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (53%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 (56%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 (59%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 (62%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 (66%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 (69%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 (72%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 (75%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 (78%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26 (81%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27 (84%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28 (88%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29 (91%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30 (94%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31 (97%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32 (100%)</t>
   </si>
 </sst>
 </file>
@@ -202,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -226,9 +127,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -555,9 +453,6 @@
       <c r="J2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -579,19 +474,16 @@
         <v>2.62</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="8" t="n">
         <v>16.46</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -614,19 +506,16 @@
         <v>2.875</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -649,19 +538,16 @@
         <v>2.32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>18.61</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -684,19 +570,16 @@
         <v>3.215</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="8" t="n">
         <v>19.44</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -719,19 +602,16 @@
         <v>3.44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -754,19 +634,16 @@
         <v>3.46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="8" t="n">
         <v>20.22</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -789,19 +666,16 @@
         <v>3.57</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="8" t="n">
         <v>15.84</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -824,19 +698,16 @@
         <v>3.19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="8" t="n">
         <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -859,19 +730,16 @@
         <v>3.15</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="8" t="n">
         <v>22.9</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -894,19 +762,16 @@
         <v>3.44</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="8" t="n">
         <v>18.3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -929,19 +794,16 @@
         <v>3.44</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -964,19 +826,16 @@
         <v>4.07</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="8" t="n">
         <v>17.4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -999,19 +858,16 @@
         <v>3.73</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="8" t="n">
         <v>17.6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -1034,19 +890,16 @@
         <v>3.78</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" s="8" t="n">
         <v>18</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -1069,19 +922,16 @@
         <v>5.25</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" s="8" t="n">
         <v>17.98</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -1104,19 +954,16 @@
         <v>5.424</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="8" t="n">
         <v>17.82</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -1139,19 +986,16 @@
         <v>5.345</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H19" s="8" t="n">
         <v>17.42</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -1174,19 +1018,16 @@
         <v>2.2</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H20" s="8" t="n">
         <v>19.47</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -1209,19 +1050,16 @@
         <v>1.615</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21" s="8" t="n">
         <v>18.52</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
@@ -1244,19 +1082,16 @@
         <v>1.835</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H22" s="8" t="n">
         <v>19.9</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
@@ -1279,19 +1114,16 @@
         <v>2.465</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H23" s="8" t="n">
         <v>20.01</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -1314,19 +1146,16 @@
         <v>3.52</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H24" s="8" t="n">
         <v>16.87</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
@@ -1349,19 +1178,16 @@
         <v>3.435</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H25" s="8" t="n">
         <v>17.3</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
@@ -1384,19 +1210,16 @@
         <v>3.84</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H26" s="8" t="n">
         <v>15.41</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
@@ -1419,19 +1242,16 @@
         <v>3.845</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H27" s="8" t="n">
         <v>17.05</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
@@ -1454,19 +1274,16 @@
         <v>1.935</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H28" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
@@ -1489,19 +1306,16 @@
         <v>2.14</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H29" s="8" t="n">
         <v>16.7</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
@@ -1524,19 +1338,16 @@
         <v>1.513</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30" s="8" t="n">
         <v>16.9</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
@@ -1559,19 +1370,16 @@
         <v>3.17</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H31" s="8" t="n">
         <v>14.5</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
@@ -1594,19 +1402,16 @@
         <v>2.77</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H32" s="8" t="n">
         <v>15.5</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
@@ -1629,19 +1434,16 @@
         <v>3.57</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H33" s="8" t="n">
         <v>14.6</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34">
@@ -1664,19 +1466,16 @@
         <v>2.78</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H34" s="8" t="n">
         <v>18.6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
@@ -1690,7 +1489,6 @@
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
-      <c r="K35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed how NA worked for build_multiple_response question, and implemented with seen_but_answered.
</commit_message>
<xml_diff>
--- a/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
+++ b/tests/testthat/_output_excel_snaps/data_to_worksheet.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">test_r_numeric</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">test_r_complex</t>
   </si>
   <si>
+    <t xml:space="preserve">test_xlr_n_percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
@@ -53,7 +56,103 @@
     <t xml:space="preserve">1+1i</t>
   </si>
   <si>
+    <t xml:space="preserve">1 (3%)</t>
+  </si>
+  <si>
     <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 (6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 (9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 (12%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 (16%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 (19%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 (22%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 (25%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 (28%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 (31%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11 (34%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 (38%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 (41%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14 (44%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 (47%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (50%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 (53%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 (56%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 (59%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 (62%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21 (66%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 (69%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 (72%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 (75%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25 (78%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26 (81%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 (84%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28 (88%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29 (91%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 (94%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31 (97%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32 (100%)</t>
   </si>
 </sst>
 </file>
@@ -103,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -127,6 +226,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -453,6 +555,9 @@
       <c r="J2" t="s">
         <v>9</v>
       </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -474,16 +579,19 @@
         <v>2.62</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="8" t="n">
         <v>16.46</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -506,16 +614,19 @@
         <v>2.875</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +649,19 @@
         <v>2.32</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>18.61</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -570,16 +684,19 @@
         <v>3.215</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="8" t="n">
         <v>19.44</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7">
@@ -602,16 +719,19 @@
         <v>3.44</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>17.02</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -634,16 +754,19 @@
         <v>3.46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="8" t="n">
         <v>20.22</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -666,16 +789,19 @@
         <v>3.57</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" s="8" t="n">
         <v>15.84</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -698,16 +824,19 @@
         <v>3.19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H10" s="8" t="n">
         <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -730,16 +859,19 @@
         <v>3.15</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="8" t="n">
         <v>22.9</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -762,16 +894,19 @@
         <v>3.44</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="8" t="n">
         <v>18.3</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -794,16 +929,19 @@
         <v>3.44</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -826,16 +964,19 @@
         <v>4.07</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H14" s="8" t="n">
         <v>17.4</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15">
@@ -858,16 +999,19 @@
         <v>3.73</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15" s="8" t="n">
         <v>17.6</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16">
@@ -890,16 +1034,19 @@
         <v>3.78</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16" s="8" t="n">
         <v>18</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17">
@@ -922,16 +1069,19 @@
         <v>5.25</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="8" t="n">
         <v>17.98</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18">
@@ -954,16 +1104,19 @@
         <v>5.424</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18" s="8" t="n">
         <v>17.82</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19">
@@ -986,16 +1139,19 @@
         <v>5.345</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="8" t="n">
         <v>17.42</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20">
@@ -1018,16 +1174,19 @@
         <v>2.2</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="8" t="n">
         <v>19.47</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="21">
@@ -1050,16 +1209,19 @@
         <v>1.615</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21" s="8" t="n">
         <v>18.52</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K21" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22">
@@ -1082,16 +1244,19 @@
         <v>1.835</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H22" s="8" t="n">
         <v>19.9</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23">
@@ -1114,16 +1279,19 @@
         <v>2.465</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H23" s="8" t="n">
         <v>20.01</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24">
@@ -1146,16 +1314,19 @@
         <v>3.52</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24" s="8" t="n">
         <v>16.87</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="25">
@@ -1178,16 +1349,19 @@
         <v>3.435</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25" s="8" t="n">
         <v>17.3</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26">
@@ -1210,16 +1384,19 @@
         <v>3.84</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H26" s="8" t="n">
         <v>15.41</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="27">
@@ -1242,16 +1419,19 @@
         <v>3.845</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H27" s="8" t="n">
         <v>17.05</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="28">
@@ -1274,16 +1454,19 @@
         <v>1.935</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H28" s="8" t="n">
         <v>18.9</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="29">
@@ -1306,16 +1489,19 @@
         <v>2.14</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29" s="8" t="n">
         <v>16.7</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30">
@@ -1338,16 +1524,19 @@
         <v>1.513</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30" s="8" t="n">
         <v>16.9</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="31">
@@ -1370,16 +1559,19 @@
         <v>3.17</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H31" s="8" t="n">
         <v>14.5</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="32">
@@ -1402,16 +1594,19 @@
         <v>2.77</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H32" s="8" t="n">
         <v>15.5</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33">
@@ -1434,16 +1629,19 @@
         <v>3.57</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H33" s="8" t="n">
         <v>14.6</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34">
@@ -1466,16 +1664,19 @@
         <v>2.78</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H34" s="8" t="n">
         <v>18.6</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="35">
@@ -1489,6 +1690,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
+      <c r="K35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>